<commit_message>
Commit before A1 is due.. wooh
</commit_message>
<xml_diff>
--- a/Assignment 1/Sample Data/Preference Distribution - Five Rounds.xlsx
+++ b/Assignment 1/Sample Data/Preference Distribution - Five Rounds.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/E09686/Teaching/ISYS1102/2023 Sem 2/Assignments/Assignment 1/sample data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rmiteduau-my.sharepoint.com/personal/s3722151_student_rmit_edu_au/Documents/2024/Semester 2/Database Applications/Assignments/DatabaseApplicationsA1/Assignment 1/Sample Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{9DB4CC4B-484C-EB4D-97E2-8C7BCD849F0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6860" yWindow="500" windowWidth="27640" windowHeight="16940" xr2:uid="{9943EECA-B431-794E-8CDE-BA29E7B687BB}"/>
+    <workbookView xWindow="20085" yWindow="-12975" windowWidth="14400" windowHeight="7290" xr2:uid="{9943EECA-B431-794E-8CDE-BA29E7B687BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -226,25 +226,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -265,9 +263,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -305,7 +303,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -411,7 +409,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -553,7 +551,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -564,20 +562,20 @@
   <dimension ref="A1:J75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
-    <col min="4" max="4" width="16.1640625" customWidth="1"/>
+    <col min="3" max="3" width="17.6875" customWidth="1"/>
+    <col min="4" max="4" width="16.1875" customWidth="1"/>
     <col min="5" max="5" width="16.5" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" customWidth="1"/>
+    <col min="6" max="6" width="15.8125" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" customWidth="1"/>
+    <col min="8" max="8" width="17.3125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -597,14 +595,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="10">
         <v>71</v>
       </c>
       <c r="D2" s="3">
@@ -619,7 +617,7 @@
       <c r="G2" s="3">
         <v>241</v>
       </c>
-      <c r="H2" s="12">
+      <c r="H2" s="11">
         <v>308</v>
       </c>
       <c r="I2">
@@ -627,75 +625,70 @@
         <v>990</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="15"/>
-      <c r="B3" s="16" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A3" s="14"/>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="13">
-        <f>C2/SUM($C2:$H2)</f>
+      <c r="C3" s="12">
+        <f t="shared" ref="C3:H3" si="0">C2/SUM($C2:$H2)</f>
         <v>7.1717171717171721E-2</v>
       </c>
-      <c r="D3" s="6">
-        <f>D2/SUM($C2:$H2)</f>
+      <c r="D3" s="1">
+        <f t="shared" si="0"/>
         <v>0.12626262626262627</v>
       </c>
-      <c r="E3" s="6">
-        <f>E2/SUM($C2:$H2)</f>
+      <c r="E3" s="1">
+        <f t="shared" si="0"/>
         <v>0.11414141414141414</v>
       </c>
-      <c r="F3" s="6">
-        <f>F2/SUM($C2:$H2)</f>
+      <c r="F3" s="1">
+        <f t="shared" si="0"/>
         <v>0.13333333333333333</v>
       </c>
-      <c r="G3" s="6">
-        <f>G2/SUM($C2:$H2)</f>
+      <c r="G3" s="1">
+        <f t="shared" si="0"/>
         <v>0.24343434343434345</v>
       </c>
-      <c r="H3" s="14">
-        <f>H2/SUM($C2:$H2)</f>
+      <c r="H3" s="13">
+        <f t="shared" si="0"/>
         <v>0.31111111111111112</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="15"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="17" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A4" s="14"/>
+      <c r="C4" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="18"/>
-    </row>
-    <row r="5" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="H4" s="16"/>
+    </row>
+    <row r="5" spans="1:10" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="9">
+      <c r="B5" s="8"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="8">
         <v>14</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="8">
         <v>21</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="8">
         <v>14</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="8">
         <v>7</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="9">
         <v>15</v>
       </c>
       <c r="J5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -705,20 +698,20 @@
         <f>D2+D5</f>
         <v>139</v>
       </c>
-      <c r="E7" s="11">
-        <f t="shared" ref="E7:H7" si="0">E2+E5</f>
+      <c r="E7" s="10">
+        <f t="shared" ref="E7:H7" si="1">E2+E5</f>
         <v>134</v>
       </c>
       <c r="F7" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>146</v>
       </c>
       <c r="G7" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>248</v>
       </c>
-      <c r="H7" s="12">
-        <f t="shared" si="0"/>
+      <c r="H7" s="11">
+        <f t="shared" si="1"/>
         <v>323</v>
       </c>
       <c r="I7">
@@ -726,63 +719,56 @@
         <v>990</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="15"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="6">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A8" s="14"/>
+      <c r="D8" s="1">
         <f>D7/SUM($C7:$H7)</f>
         <v>0.14040404040404039</v>
       </c>
-      <c r="E8" s="13">
-        <f t="shared" ref="E8:H8" si="1">E7/SUM($C7:$H7)</f>
+      <c r="E8" s="12">
+        <f t="shared" ref="E8:H8" si="2">E7/SUM($C7:$H7)</f>
         <v>0.13535353535353536</v>
       </c>
-      <c r="F8" s="6">
-        <f t="shared" si="1"/>
+      <c r="F8" s="1">
+        <f t="shared" si="2"/>
         <v>0.14747474747474748</v>
       </c>
-      <c r="G8" s="6">
-        <f t="shared" si="1"/>
+      <c r="G8" s="1">
+        <f t="shared" si="2"/>
         <v>0.25050505050505051</v>
       </c>
-      <c r="H8" s="14">
-        <f t="shared" si="1"/>
+      <c r="H8" s="13">
+        <f t="shared" si="2"/>
         <v>0.32626262626262625</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="15"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="17" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A9" s="14"/>
+      <c r="E9" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="18"/>
-    </row>
-    <row r="10" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="H9" s="16"/>
+    </row>
+    <row r="10" spans="1:10" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9">
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8">
         <f>22+5+5</f>
         <v>32</v>
       </c>
-      <c r="E10" s="19"/>
-      <c r="F10" s="9">
+      <c r="E10" s="17"/>
+      <c r="F10" s="8">
         <f>26+7+8</f>
         <v>41</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="8">
         <f>18+2+3</f>
         <v>23</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H10" s="9">
         <f>24+7+7</f>
         <v>38</v>
       </c>
@@ -794,14 +780,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="11">
+      <c r="D12" s="10">
         <f>D7+D10</f>
         <v>171</v>
       </c>
@@ -814,7 +800,7 @@
         <f>G7+G10</f>
         <v>271</v>
       </c>
-      <c r="H12" s="12">
+      <c r="H12" s="11">
         <f>H7+H10</f>
         <v>361</v>
       </c>
@@ -823,57 +809,49 @@
         <v>990</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A13" s="5"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="13">
+      <c r="D13" s="12">
         <f>D12/SUM($C12:$H12)</f>
         <v>0.17272727272727273</v>
       </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6">
+      <c r="F13" s="1">
         <f>F12/SUM($C12:$H12)</f>
         <v>0.18888888888888888</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="1">
         <f>G12/SUM($C12:$H12)</f>
         <v>0.27373737373737372</v>
       </c>
-      <c r="H13" s="14">
+      <c r="H13" s="13">
         <f>H12/SUM($C12:$H12)</f>
         <v>0.36464646464646466</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="15"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="17" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A14" s="14"/>
+      <c r="D14" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="18"/>
-    </row>
-    <row r="15" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="H14" s="16"/>
+    </row>
+    <row r="15" spans="1:10" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9">
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8">
         <f>28+6+4+10+1+6+0+8+0+0</f>
         <v>63</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G15" s="8">
         <f>14+4+2+1+0+6+0+3+0+0</f>
         <v>30</v>
       </c>
-      <c r="H15" s="10">
+      <c r="H15" s="9">
         <f>33+9+0+8+5+8+2+7+5+1</f>
         <v>78</v>
       </c>
@@ -885,8 +863,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
@@ -894,7 +872,7 @@
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
-      <c r="F17" s="11">
+      <c r="F17" s="10">
         <f>F12+F15</f>
         <v>250</v>
       </c>
@@ -902,7 +880,7 @@
         <f>G12+G15</f>
         <v>301</v>
       </c>
-      <c r="H17" s="12">
+      <c r="H17" s="11">
         <f>H12+H15</f>
         <v>439</v>
       </c>
@@ -911,58 +889,49 @@
         <v>990</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A18" s="5"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="13">
+      <c r="F18" s="12">
         <f>F17/SUM($F17:$H17)</f>
         <v>0.25252525252525254</v>
       </c>
-      <c r="G18" s="6">
-        <f t="shared" ref="G18:H18" si="2">G17/SUM($F17:$H17)</f>
+      <c r="G18" s="1">
+        <f t="shared" ref="G18:H18" si="3">G17/SUM($F17:$H17)</f>
         <v>0.30404040404040406</v>
       </c>
-      <c r="H18" s="14">
-        <f t="shared" si="2"/>
+      <c r="H18" s="13">
+        <f t="shared" si="3"/>
         <v>0.44343434343434346</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="15"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="17" t="s">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A19" s="14"/>
+      <c r="F19" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="G19" s="16"/>
-      <c r="H19" s="18"/>
-    </row>
-    <row r="20" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
+      <c r="H19" s="16"/>
+    </row>
+    <row r="20" spans="1:10" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9">
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8">
         <v>131</v>
       </c>
-      <c r="H20" s="10">
+      <c r="H20" s="9">
         <v>145</v>
       </c>
       <c r="J20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A23" s="2" t="s">
         <v>19</v>
       </c>
@@ -987,33 +956,28 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A24" s="5"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6">
+      <c r="G24" s="1">
         <f>G23/SUM($G23:$H23)</f>
         <v>0.42519685039370081</v>
       </c>
-      <c r="H24" s="7">
+      <c r="H24" s="6">
         <f>H23/SUM($G23:$H23)</f>
         <v>0.57480314960629919</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="10"/>
-    </row>
-    <row r="74" spans="7:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="7"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="9"/>
+    </row>
+    <row r="74" spans="7:8" x14ac:dyDescent="0.5">
       <c r="G74">
         <v>1</v>
       </c>
@@ -1021,7 +985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="7:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="7:8" x14ac:dyDescent="0.5">
       <c r="G75">
         <v>0</v>
       </c>
@@ -1031,7 +995,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Calibri"&amp;12&amp;KEEDC00 RMIT Classification: Trusted&amp;1#_x000D_</oddHeader>
   </headerFooter>

</xml_diff>